<commit_message>
Track fuel-cost-driven changes in cargo dist transported down to the vehicle technology (engine type) level (#6)
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Repositories\eps-us\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="SoCDTtiNTY" sheetId="2" r:id="rId2"/>
+    <sheet name="SoCDTtiNTY-psgr" sheetId="2" r:id="rId2"/>
+    <sheet name="SoCDTtiNTY-frgt" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>SoCDTtiNTY Share of Cargo Dist Transported that is New This Year</t>
   </si>
@@ -76,13 +77,28 @@
     <t>motorbikes</t>
   </si>
   <si>
-    <t>passenger</t>
-  </si>
-  <si>
-    <t>freight</t>
-  </si>
-  <si>
     <t>Share that is New (dimensionless)</t>
+  </si>
+  <si>
+    <t>battery electric vehicle</t>
+  </si>
+  <si>
+    <t>natural gas vehicle</t>
+  </si>
+  <si>
+    <t>gasoline vehicle</t>
+  </si>
+  <si>
+    <t>diesel vehicle</t>
+  </si>
+  <si>
+    <t>plugin hybrid vehicle</t>
+  </si>
+  <si>
+    <t>LPG vehicle</t>
+  </si>
+  <si>
+    <t>hydrogen vehicle</t>
   </si>
 </sst>
 </file>
@@ -126,13 +142,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -513,29 +532,43 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -543,10 +576,25 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="C2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="D2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="H2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -554,10 +602,25 @@
         <v>4.3499999999999997E-2</v>
       </c>
       <c r="C3">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="D3">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="F3">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="G3">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="H3">
+        <v>4.3499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -565,10 +628,25 @@
         <v>4.1599999999999998E-2</v>
       </c>
       <c r="C4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="D4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="E4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="G4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="H4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -578,8 +656,23 @@
       <c r="C5">
         <v>2.9000000000000001E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -587,10 +680,25 @@
         <v>2.9819999999999999E-2</v>
       </c>
       <c r="C6">
-        <v>3.0300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="F6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="H6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -598,6 +706,223 @@
         <v>5.8700000000000002E-2</v>
       </c>
       <c r="C7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="D7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="E7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="F7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="G7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="H7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="G4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="E6">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="G6">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="H6">
+        <v>3.0300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Additional transportation calibration edits
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7068EE-DE0D-4380-BEB0-F0EE695126AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="21075" windowHeight="10050"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SoCDTtiNTY-psgr" sheetId="2" r:id="rId2"/>
     <sheet name="SoCDTtiNTY-frgt" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -104,7 +116,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -247,6 +259,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -282,6 +311,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,19 +503,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -477,47 +523,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -528,7 +574,211 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
+    <col min="2" max="8" width="14.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="C2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="E2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="F2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="G2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="H2">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>0.09</v>
+      </c>
+      <c r="C3">
+        <v>0.09</v>
+      </c>
+      <c r="D3">
+        <v>0.09</v>
+      </c>
+      <c r="E3">
+        <v>0.09</v>
+      </c>
+      <c r="F3">
+        <v>0.09</v>
+      </c>
+      <c r="G3">
+        <v>0.09</v>
+      </c>
+      <c r="H3">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="D4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="E4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="G4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="H4">
+        <v>4.1599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="H5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="F6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+      <c r="H6">
+        <v>2.9819999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="C7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="D7">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="F7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="G7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="H7">
+        <v>5.8700000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -538,13 +788,13 @@
       <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.1328125" customWidth="1"/>
-    <col min="2" max="8" width="14.3984375" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
+    <col min="2" max="8" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -570,85 +820,85 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>7.5999999999999998E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="C2">
-        <v>7.5999999999999998E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D2">
-        <v>7.8E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="E2">
-        <v>7.5999999999999998E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="F2">
-        <v>7.5999999999999998E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="G2">
-        <v>7.5999999999999998E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="H2">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>4.2700000000000002E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="C3">
-        <v>4.2700000000000002E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="D3">
-        <v>4.2700000000000002E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="E3">
-        <v>4.2700000000000002E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="F3">
-        <v>4.2700000000000002E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="G3">
-        <v>4.2700000000000002E-2</v>
+        <v>3.5499999999999997E-2</v>
       </c>
       <c r="H3">
-        <v>4.2700000000000002E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+        <v>3.5499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>4.1599999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="C4">
-        <v>4.1599999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D4">
-        <v>4.1599999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="E4">
-        <v>4.1599999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F4">
-        <v>4.1599999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="G4">
-        <v>4.1599999999999998E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="H4">
-        <v>4.1599999999999998E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -674,215 +924,11 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-      <c r="C6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-      <c r="D6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-      <c r="E6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-      <c r="F6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-      <c r="G6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-      <c r="H6">
-        <v>2.9819999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>5.8700000000000002E-2</v>
-      </c>
-      <c r="C7">
-        <v>5.8700000000000002E-2</v>
-      </c>
-      <c r="D7">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="E7">
-        <v>5.8700000000000002E-2</v>
-      </c>
-      <c r="F7">
-        <v>5.8700000000000002E-2</v>
-      </c>
-      <c r="G7">
-        <v>5.8700000000000002E-2</v>
-      </c>
-      <c r="H7">
-        <v>5.8700000000000002E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="19.1328125" customWidth="1"/>
-    <col min="2" max="8" width="14.3984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="C2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="D2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="E2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="F2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="G2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="H2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="C3">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="D3">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="E3">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="F3">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="G3">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="H3">
-        <v>3.5499999999999997E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="C4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="D4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="E4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="F4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="G4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="H4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="C5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="D5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="E5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="G5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="H5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
         <v>3.0300000000000001E-2</v>
       </c>
       <c r="C6">
@@ -904,7 +950,7 @@
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Updates to AVL and SOCDtINtY to align sales data.
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73732797-F0D5-4552-9011-A59D9397727A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE1583E-2085-4BE7-B456-43253B7BD58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -506,16 +506,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -523,47 +525,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -581,16 +583,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" customWidth="1"/>
-    <col min="2" max="8" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -616,33 +618,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>8.5999999999999993E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="C2">
-        <v>8.5999999999999993E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D2">
-        <v>8.5999999999999993E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E2">
-        <v>8.5999999999999993E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F2">
-        <v>8.5999999999999993E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="G2">
-        <v>8.5999999999999993E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="H2">
-        <v>8.5999999999999993E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -668,7 +670,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -694,7 +696,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -720,7 +722,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -746,7 +748,7 @@
         <v>2.9819999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -785,16 +787,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H4"/>
+      <selection activeCell="B3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" customWidth="1"/>
-    <col min="2" max="8" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -820,7 +822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -846,33 +848,33 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>3.5499999999999997E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="C3">
-        <v>3.5499999999999997E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="D3">
-        <v>3.5499999999999997E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="E3">
-        <v>3.5499999999999997E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="F3">
-        <v>3.5499999999999997E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="G3">
-        <v>3.5499999999999997E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="H3">
-        <v>3.5499999999999997E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>5.7500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -898,7 +900,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -924,7 +926,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -950,7 +952,7 @@
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Additional transportation calibration edits to adjust psgr LDV lifetime and moving TTS s-curve for BEVs to reach 1 by 2035
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE1583E-2085-4BE7-B456-43253B7BD58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC30D8DD-9E3D-47D4-B288-7FFFA9B36699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -224,9 +224,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,26 +259,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,26 +294,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -506,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -582,8 +548,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,25 +589,32 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>6.5000000000000002E-2</v>
+        <f>1/20</f>
+        <v>0.05</v>
       </c>
       <c r="C2">
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" ref="C2:H2" si="0">1/20</f>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="E2">
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="F2">
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="G2">
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="H2">
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update passenger LDV lifetime to better match historical US sales
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC30D8DD-9E3D-47D4-B288-7FFFA9B36699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6E853D-967A-4A7D-929E-2E57C99CC705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,14 +476,14 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -491,47 +491,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -549,16 +549,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -584,40 +584,40 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <f>1/20</f>
-        <v>0.05</v>
+        <f>1/17</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:H2" si="0">1/20</f>
-        <v>0.05</v>
+        <f t="shared" ref="C2:H2" si="0">1/17</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="D2">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -643,7 +643,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -669,7 +669,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -695,7 +695,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -721,7 +721,7 @@
         <v>2.9819999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -763,13 +763,13 @@
       <selection activeCell="B3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -795,7 +795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -821,7 +821,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -847,7 +847,7 @@
         <v>5.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -873,7 +873,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -899,7 +899,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -925,7 +925,7 @@
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Fix to discontinuity in motorbikes data
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\SoCDTtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6E853D-967A-4A7D-929E-2E57C99CC705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B572B393-2293-47FB-8029-7D485036E872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -476,14 +476,14 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -491,47 +491,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -549,16 +549,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -584,7 +584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -617,7 +617,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -643,7 +643,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -669,7 +669,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -695,7 +695,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -721,30 +721,30 @@
         <v>2.9819999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
-        <v>5.8700000000000002E-2</v>
+        <v>5.8500000000000003E-2</v>
       </c>
       <c r="C7">
-        <v>5.8700000000000002E-2</v>
+        <v>5.8500000000000003E-2</v>
       </c>
       <c r="D7">
-        <v>6.8000000000000005E-2</v>
+        <v>5.8500000000000003E-2</v>
       </c>
       <c r="E7">
-        <v>5.8700000000000002E-2</v>
+        <v>5.8500000000000003E-2</v>
       </c>
       <c r="F7">
-        <v>5.8700000000000002E-2</v>
+        <v>5.8500000000000003E-2</v>
       </c>
       <c r="G7">
-        <v>5.8700000000000002E-2</v>
+        <v>5.8500000000000003E-2</v>
       </c>
       <c r="H7">
-        <v>5.8700000000000002E-2</v>
+        <v>5.8500000000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -763,13 +763,13 @@
       <selection activeCell="B3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -795,7 +795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -821,7 +821,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -847,7 +847,7 @@
         <v>5.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -873,7 +873,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -899,7 +899,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -925,7 +925,7 @@
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Align SoCDTtiNTY for freight trucks with AVL values
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B572B393-2293-47FB-8029-7D485036E872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B539881-35F2-4ACF-93AE-EB11A251A4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -548,7 +548,7 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
@@ -760,7 +760,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H3"/>
+      <selection activeCell="B2" sqref="B2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,25 +800,32 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>7.1999999999999995E-2</v>
+        <f>1/17</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="C2">
-        <v>7.1999999999999995E-2</v>
+        <f t="shared" ref="C2:H2" si="0">1/17</f>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="D2">
-        <v>7.1999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="E2">
-        <v>7.1999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="F2">
-        <v>7.1999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="G2">
-        <v>7.1999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="H2">
-        <v>7.1999999999999995E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -826,25 +833,32 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>5.7500000000000002E-2</v>
+        <f>1/19</f>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="C3">
-        <v>5.7500000000000002E-2</v>
+        <f t="shared" ref="C3:H3" si="1">1/19</f>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="D3">
-        <v>5.7500000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="E3">
-        <v>5.7500000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="F3">
-        <v>5.7500000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="G3">
-        <v>5.7500000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="H3">
-        <v>5.7500000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.2631578947368418E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>